<commit_message>
Updated missing three-equation models
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88C6A94-D887-40DF-9983-E54350B19BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975FC861-3544-4AD0-82DE-06FA4F4F4918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-12660" windowWidth="16410" windowHeight="12660" firstSheet="7" activeTab="8" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="7" activeTab="8" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="occupation_numbers" sheetId="11" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="222">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1060,7 +1060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1172,6 +1172,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1187,54 +1212,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1862,20 +1856,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -2367,7 +2361,7 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:D19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -2381,31 +2375,30 @@
     <col min="4" max="4" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="64" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="79" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="80"/>
-    </row>
-    <row r="4" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="59" t="s">
+      <c r="B3" s="64"/>
+    </row>
+    <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="76"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
@@ -2419,7 +2412,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
@@ -2433,7 +2426,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>217</v>
       </c>
@@ -2447,7 +2440,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>180</v>
       </c>
@@ -2461,7 +2454,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>33</v>
       </c>
@@ -2475,7 +2468,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>197</v>
       </c>
@@ -2489,7 +2482,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>34</v>
       </c>
@@ -2503,7 +2496,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>39</v>
       </c>
@@ -2517,7 +2510,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>166</v>
       </c>
@@ -2531,7 +2524,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>35</v>
       </c>
@@ -2545,7 +2538,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>218</v>
       </c>
@@ -2615,51 +2608,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="66" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="H1" s="77" t="s">
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="H1" s="66" t="s">
         <v>212</v>
       </c>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="N1" s="77" t="s">
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="N1" s="66" t="s">
         <v>213</v>
       </c>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="H2" s="74" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="H2" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="74" t="s">
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="N2" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
     </row>
     <row r="3" spans="2:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -2688,16 +2680,16 @@
       <c r="L3" s="4">
         <v>2017</v>
       </c>
-      <c r="O3" s="73">
+      <c r="O3" s="61">
         <v>2001</v>
       </c>
-      <c r="P3" s="73">
+      <c r="P3" s="61">
         <v>2006</v>
       </c>
       <c r="Q3" s="4">
         <v>2012</v>
       </c>
-      <c r="R3" s="73">
+      <c r="R3" s="61">
         <v>2017</v>
       </c>
     </row>
@@ -2844,7 +2836,7 @@
       <c r="R6" s="30">
         <v>7088689</v>
       </c>
-      <c r="U6" s="78"/>
+      <c r="U6" s="62"/>
     </row>
     <row r="7" spans="2:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
@@ -2949,59 +2941,59 @@
       <c r="B10" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="72">
+      <c r="C10" s="60">
         <f>+C4/C$7</f>
         <v>0.45714984615740595</v>
       </c>
-      <c r="D10" s="72">
+      <c r="D10" s="60">
         <f t="shared" ref="D10:F10" si="3">+D4/D$7</f>
         <v>0.41709555692655492</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="60">
         <f t="shared" si="3"/>
         <v>0.34020945227600013</v>
       </c>
-      <c r="F10" s="72">
+      <c r="F10" s="60">
         <f t="shared" si="3"/>
         <v>0.30283992492425504</v>
       </c>
       <c r="H10" t="s">
         <v>93</v>
       </c>
-      <c r="I10" s="72">
-        <f>+I4/I$7</f>
+      <c r="I10" s="60">
+        <f t="shared" ref="I10:L13" si="4">+I4/I$7</f>
         <v>0.4711448608360938</v>
       </c>
-      <c r="J10" s="72">
-        <f>+J4/J$7</f>
+      <c r="J10" s="60">
+        <f t="shared" si="4"/>
         <v>0.43293416841828847</v>
       </c>
-      <c r="K10" s="72">
-        <f>+K4/K$7</f>
+      <c r="K10" s="60">
+        <f t="shared" si="4"/>
         <v>0.34955936030966289</v>
       </c>
-      <c r="L10" s="72">
-        <f>+L4/L$7</f>
+      <c r="L10" s="60">
+        <f t="shared" si="4"/>
         <v>0.31351916949490627</v>
       </c>
-      <c r="M10" s="72"/>
+      <c r="M10" s="60"/>
       <c r="N10" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="72">
+      <c r="O10" s="60">
         <f>+O4/O$7</f>
         <v>0.48978827880706949</v>
       </c>
-      <c r="P10" s="72">
-        <f t="shared" ref="P10:R10" si="4">+P4/P$7</f>
+      <c r="P10" s="60">
+        <f t="shared" ref="P10:R10" si="5">+P4/P$7</f>
         <v>0.45247370296325407</v>
       </c>
-      <c r="Q10" s="72">
-        <f t="shared" si="4"/>
+      <c r="Q10" s="60">
+        <f t="shared" si="5"/>
         <v>0.36498720813961988</v>
       </c>
-      <c r="R10" s="72">
-        <f t="shared" si="4"/>
+      <c r="R10" s="60">
+        <f t="shared" si="5"/>
         <v>0.32667469189840564</v>
       </c>
     </row>
@@ -3009,59 +3001,59 @@
       <c r="B11" t="s">
         <v>211</v>
       </c>
-      <c r="C11" s="72">
-        <f t="shared" ref="C11:F11" si="5">+C5/C$7</f>
+      <c r="C11" s="60">
+        <f t="shared" ref="C11:F11" si="6">+C5/C$7</f>
         <v>0.23196623561416246</v>
       </c>
-      <c r="D11" s="72">
-        <f t="shared" si="5"/>
+      <c r="D11" s="60">
+        <f t="shared" si="6"/>
         <v>0.22465000720331807</v>
       </c>
-      <c r="E11" s="72">
-        <f t="shared" si="5"/>
+      <c r="E11" s="60">
+        <f t="shared" si="6"/>
         <v>0.2208193959779306</v>
       </c>
-      <c r="F11" s="72">
-        <f t="shared" si="5"/>
+      <c r="F11" s="60">
+        <f t="shared" si="6"/>
         <v>0.2201646387778057</v>
       </c>
       <c r="H11" t="s">
         <v>211</v>
       </c>
-      <c r="I11" s="72">
-        <f>+I5/I$7</f>
+      <c r="I11" s="60">
+        <f t="shared" si="4"/>
         <v>0.24976687212837287</v>
       </c>
-      <c r="J11" s="72">
-        <f>+J5/J$7</f>
+      <c r="J11" s="60">
+        <f t="shared" si="4"/>
         <v>0.24347895838928746</v>
       </c>
-      <c r="K11" s="72">
-        <f>+K5/K$7</f>
+      <c r="K11" s="60">
+        <f t="shared" si="4"/>
         <v>0.23955194574798333</v>
       </c>
-      <c r="L11" s="72">
-        <f>+L5/L$7</f>
+      <c r="L11" s="60">
+        <f t="shared" si="4"/>
         <v>0.24000992639179192</v>
       </c>
-      <c r="M11" s="72"/>
+      <c r="M11" s="60"/>
       <c r="N11" t="s">
         <v>211</v>
       </c>
-      <c r="O11" s="72">
-        <f t="shared" ref="O11:R13" si="6">+O5/O$7</f>
+      <c r="O11" s="60">
+        <f t="shared" ref="O11:R13" si="7">+O5/O$7</f>
         <v>0.27152068520708916</v>
       </c>
-      <c r="P11" s="72">
-        <f t="shared" si="6"/>
+      <c r="P11" s="60">
+        <f t="shared" si="7"/>
         <v>0.26756261071145815</v>
       </c>
-      <c r="Q11" s="72">
-        <f t="shared" si="6"/>
+      <c r="Q11" s="60">
+        <f t="shared" si="7"/>
         <v>0.26720187616885743</v>
       </c>
-      <c r="R11" s="72">
-        <f t="shared" si="6"/>
+      <c r="R11" s="60">
+        <f t="shared" si="7"/>
         <v>0.26624316934555964</v>
       </c>
     </row>
@@ -3069,59 +3061,59 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="72">
-        <f t="shared" ref="C12:F12" si="7">+C6/C$7</f>
+      <c r="C12" s="60">
+        <f t="shared" ref="C12:F12" si="8">+C6/C$7</f>
         <v>0.31088391822843159</v>
       </c>
-      <c r="D12" s="72">
-        <f t="shared" si="7"/>
+      <c r="D12" s="60">
+        <f t="shared" si="8"/>
         <v>0.35825443587012701</v>
       </c>
-      <c r="E12" s="72">
-        <f t="shared" si="7"/>
+      <c r="E12" s="60">
+        <f t="shared" si="8"/>
         <v>0.43897115174606927</v>
       </c>
-      <c r="F12" s="72">
-        <f t="shared" si="7"/>
+      <c r="F12" s="60">
+        <f t="shared" si="8"/>
         <v>0.47699543629793922</v>
       </c>
       <c r="H12" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="72">
-        <f>+I6/I$7</f>
+      <c r="I12" s="60">
+        <f t="shared" si="4"/>
         <v>0.2790882670355333</v>
       </c>
-      <c r="J12" s="72">
-        <f>+J6/J$7</f>
+      <c r="J12" s="60">
+        <f t="shared" si="4"/>
         <v>0.32358687319242407</v>
       </c>
-      <c r="K12" s="72">
-        <f>+K6/K$7</f>
+      <c r="K12" s="60">
+        <f t="shared" si="4"/>
         <v>0.41088869394235378</v>
       </c>
-      <c r="L12" s="72">
-        <f>+L6/L$7</f>
+      <c r="L12" s="60">
+        <f t="shared" si="4"/>
         <v>0.44647090411330181</v>
       </c>
-      <c r="M12" s="72"/>
+      <c r="M12" s="60"/>
       <c r="N12" t="s">
         <v>10</v>
       </c>
-      <c r="O12" s="72">
-        <f t="shared" si="6"/>
+      <c r="O12" s="60">
+        <f t="shared" si="7"/>
         <v>0.23869103598584135</v>
       </c>
-      <c r="P12" s="72">
-        <f t="shared" si="6"/>
+      <c r="P12" s="60">
+        <f t="shared" si="7"/>
         <v>0.27996368632528773</v>
       </c>
-      <c r="Q12" s="72">
-        <f t="shared" si="6"/>
+      <c r="Q12" s="60">
+        <f t="shared" si="7"/>
         <v>0.36781091569152263</v>
       </c>
-      <c r="R12" s="72">
-        <f t="shared" si="6"/>
+      <c r="R12" s="60">
+        <f t="shared" si="7"/>
         <v>0.40708213875603472</v>
       </c>
     </row>
@@ -3129,59 +3121,59 @@
       <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="72">
-        <f t="shared" ref="C13:F13" si="8">+C7/C$7</f>
+      <c r="C13" s="60">
+        <f t="shared" ref="C13:F13" si="9">+C7/C$7</f>
         <v>1</v>
       </c>
-      <c r="D13" s="72">
-        <f t="shared" si="8"/>
+      <c r="D13" s="60">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="E13" s="72">
-        <f t="shared" si="8"/>
+      <c r="E13" s="60">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="F13" s="72">
-        <f t="shared" si="8"/>
+      <c r="F13" s="60">
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="H13" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="72">
-        <f>+I7/I$7</f>
+      <c r="I13" s="60">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="J13" s="72">
-        <f>+J7/J$7</f>
+      <c r="J13" s="60">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="K13" s="72">
-        <f>+K7/K$7</f>
+      <c r="K13" s="60">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="L13" s="72">
-        <f>+L7/L$7</f>
+      <c r="L13" s="60">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M13" s="72"/>
+      <c r="M13" s="60"/>
       <c r="N13" t="s">
         <v>71</v>
       </c>
-      <c r="O13" s="72">
-        <f t="shared" si="6"/>
+      <c r="O13" s="60">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P13" s="72">
-        <f t="shared" si="6"/>
+      <c r="P13" s="60">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q13" s="72">
-        <f t="shared" si="6"/>
+      <c r="Q13" s="60">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="R13" s="72">
-        <f t="shared" si="6"/>
+      <c r="R13" s="60">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -3222,16 +3214,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="70"/>
+      <c r="C2" s="69"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B3" s="71" t="s">
+      <c r="B3" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="59" t="s">
         <v>208</v>
       </c>
     </row>
@@ -3524,10 +3516,10 @@
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="71" t="s">
+      <c r="B40" t="s">
         <v>180</v>
       </c>
-      <c r="C40" s="71" t="s">
+      <c r="C40" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3596,10 +3588,10 @@
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="71" t="s">
+      <c r="B49" t="s">
         <v>188</v>
       </c>
-      <c r="C49" s="71" t="s">
+      <c r="C49" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3760,13 +3752,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3880,12 +3872,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -4184,12 +4176,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -4515,21 +4507,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="63" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -4767,13 +4759,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="62" t="s">
+      <c r="A21" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="51"/>
@@ -4783,10 +4775,10 @@
       <c r="E22" s="51"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="79" t="s">
+      <c r="B23" s="63" t="s">
         <v>143</v>
       </c>
       <c r="C23" s="51"/>
@@ -4801,13 +4793,13 @@
       <c r="E24" s="51"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="61" t="s">
+      <c r="A25" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -5069,13 +5061,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="62" t="s">
+      <c r="A43" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="62"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="62"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -5111,10 +5103,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="64" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5429,10 +5421,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="64" t="s">
         <v>143</v>
       </c>
     </row>
@@ -5443,36 +5435,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="74"/>
+      <c r="U3" s="74"/>
+      <c r="V3" s="74"/>
+      <c r="W3" s="74"/>
+      <c r="X3" s="74"/>
+      <c r="Y3" s="74"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -5897,19 +5889,19 @@
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="80">
+      <c r="B14" s="64">
         <v>156</v>
       </c>
       <c r="T14" s="4"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="B15" s="80">
+      <c r="B15" s="64">
         <v>16720</v>
       </c>
       <c r="T15" s="4"/>
@@ -5936,55 +5928,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="65" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="82">
+      <c r="B2" s="65">
         <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" s="83"/>
-      <c r="B3" s="84"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="68" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="67" t="s">
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="81" t="s">
+      <c r="L4" s="75"/>
+      <c r="M4" s="75"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
+      <c r="P4" s="76"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76"/>
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="76"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">
@@ -7086,10 +7078,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A38" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:E45"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7099,20 +7091,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -7261,20 +7253,20 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="80"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="79"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
@@ -7360,7 +7352,7 @@
         <v>8.2404717945099751E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="19" t="s">
         <v>10</v>
       </c>
@@ -7389,7 +7381,7 @@
         <v>8.992433008205325E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>140</v>
       </c>
@@ -7397,7 +7389,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -7414,7 +7406,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>118</v>
       </c>
@@ -7425,23 +7417,23 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="65" t="s">
+    <row r="23" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G24" s="64" t="s">
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G24" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
@@ -7466,106 +7458,139 @@
       <c r="I25" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>0.28989378675668298</v>
+      </c>
+      <c r="M25">
+        <v>0.31427353528921897</v>
+      </c>
+      <c r="N25">
+        <v>0.78279708146500204</v>
+      </c>
+      <c r="O25">
+        <v>0.24817665064047001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
       <c r="B26" s="9">
-        <v>0.28653203408786099</v>
+        <v>0.28989378675668298</v>
       </c>
       <c r="C26" s="9">
-        <v>0.432813593737364</v>
+        <v>0.31427353528921897</v>
       </c>
       <c r="D26" s="9">
-        <v>0.72863646579924202</v>
+        <v>0.78279708146500204</v>
       </c>
       <c r="E26" s="9">
-        <v>0.13590170492659701</v>
+        <v>0.24817665064047001</v>
       </c>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="3">+C26/$B26</f>
-        <v>1.5105242773820111</v>
+        <v>1.0840988998256753</v>
       </c>
       <c r="H26" s="18">
         <f t="shared" si="3"/>
-        <v>2.5429494057052482</v>
+        <v>2.7002892687797702</v>
       </c>
       <c r="I26" s="18">
         <f t="shared" si="3"/>
-        <v>0.47429846843904605</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.85609510095769148</v>
+      </c>
+      <c r="L26">
+        <v>0.218265282529087</v>
+      </c>
+      <c r="M26">
+        <v>0.494405218087976</v>
+      </c>
+      <c r="N26">
+        <v>0.78588256241046905</v>
+      </c>
+      <c r="O26">
+        <v>3.5119315719301103E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="9">
-        <v>0.276932075864669</v>
+        <v>0.218265282529087</v>
       </c>
       <c r="C27" s="9">
-        <v>0.57770093297611302</v>
+        <v>0.494405218087976</v>
       </c>
       <c r="D27" s="9">
-        <v>0.59045981810458203</v>
+        <v>0.78588256241046905</v>
       </c>
       <c r="E27" s="9">
-        <v>0.11649908855437099</v>
+        <v>3.5119315719301103E-2</v>
       </c>
       <c r="G27" s="18">
         <f t="shared" si="3"/>
-        <v>2.0860744685221064</v>
+        <v>2.2651573917720484</v>
       </c>
       <c r="H27" s="18">
         <f t="shared" si="3"/>
-        <v>2.1321467232027236</v>
+        <v>3.6005843591077697</v>
       </c>
       <c r="I27" s="18">
         <f t="shared" si="3"/>
-        <v>0.42067748270265992</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.16090197814497112</v>
+      </c>
+      <c r="L27">
+        <v>0.24165677019192</v>
+      </c>
+      <c r="M27">
+        <v>1.0090544996103099</v>
+      </c>
+      <c r="N27">
+        <v>0.15247236045851001</v>
+      </c>
+      <c r="O27">
+        <v>9.3186362566577502E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="20">
-        <v>0.26284326769114302</v>
+        <v>0.24165677019192</v>
       </c>
       <c r="C28" s="20">
-        <v>0.69281313851899595</v>
+        <v>1.0090544996103099</v>
       </c>
       <c r="D28" s="20">
-        <v>0.46538756699114298</v>
+        <v>0.15247236045851001</v>
       </c>
       <c r="E28" s="20">
-        <v>8.4193690103555402E-2</v>
+        <v>9.3186362566577502E-2</v>
       </c>
       <c r="G28" s="18">
         <f t="shared" si="3"/>
-        <v>2.635841292815968</v>
+        <v>4.1755689228525847</v>
       </c>
       <c r="H28" s="18">
         <f t="shared" si="3"/>
-        <v>1.7705896410403859</v>
+        <v>0.63094595006553655</v>
       </c>
       <c r="I28" s="18">
         <f t="shared" si="3"/>
-        <v>0.32031899026034083</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>0.38561453292854309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>140</v>
       </c>
       <c r="B30" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>19</v>
       </c>
@@ -7582,7 +7607,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>118</v>
       </c>
@@ -7601,20 +7626,20 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="65" t="s">
+      <c r="A34" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="65"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G35" s="64" t="s">
+      <c r="G35" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
     </row>
     <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
@@ -7745,20 +7770,20 @@
       <c r="E43" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="65" t="s">
+      <c r="A45" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
+      <c r="B45" s="80"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="80"/>
     </row>
     <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G46" s="64" t="s">
+      <c r="G46" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="79"/>
     </row>
     <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="10" t="s">

</xml_diff>

<commit_message>
Started draft of data appendix
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8E5A75-70EC-492F-8289-58B0E03BA7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0246BD-C8A3-461C-8F5F-7360570B1F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="-25230" windowWidth="16410" windowHeight="12675" firstSheet="8" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="28695" yWindow="-12660" windowWidth="16410" windowHeight="12660" tabRatio="656" firstSheet="9" activeTab="12" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="occupation_numbers" sheetId="11" r:id="rId1"/>
@@ -25,7 +25,11 @@
     <sheet name="OLS_thetas" sheetId="8" r:id="rId10"/>
     <sheet name="sigma_estimates" sheetId="3" r:id="rId11"/>
     <sheet name="top_jobs_skill" sheetId="5" r:id="rId12"/>
+    <sheet name="index_composition" sheetId="14" r:id="rId13"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId14"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'step-up'!$E$9:$F$32</definedName>
   </definedNames>
@@ -94,26 +98,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={89256DDE-9554-499E-A7D9-CD9CC41B184F}</author>
-  </authors>
-  <commentList>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{89256DDE-9554-499E-A7D9-CD9CC41B184F}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Should I winsorize it?</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="245">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -801,6 +787,78 @@
   <si>
     <t>9211 post wrkr, mail sort, msngr, courir</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Name in SES</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>chands</t>
+  </si>
+  <si>
+    <t>cstamina</t>
+  </si>
+  <si>
+    <t>cpeople</t>
+  </si>
+  <si>
+    <t>cteamwk</t>
+  </si>
+  <si>
+    <t>clisten</t>
+  </si>
+  <si>
+    <t>bvariety</t>
+  </si>
+  <si>
+    <t>cspeech</t>
+  </si>
+  <si>
+    <t>cpersuad</t>
+  </si>
+  <si>
+    <t>cteach</t>
+  </si>
+  <si>
+    <t>brepeat</t>
+  </si>
+  <si>
+    <t>bme4</t>
+  </si>
+  <si>
+    <t>cwritelg</t>
+  </si>
+  <si>
+    <t>clong</t>
+  </si>
+  <si>
+    <t>ccalca</t>
+  </si>
+  <si>
+    <t>cpercent</t>
+  </si>
+  <si>
+    <t>cstats</t>
+  </si>
+  <si>
+    <t>csolutn</t>
+  </si>
+  <si>
+    <t>canalyse</t>
+  </si>
+  <si>
+    <t>cstrengt</t>
+  </si>
+  <si>
+    <t>cplanme</t>
+  </si>
+  <si>
+    <t>cplanoth</t>
+  </si>
 </sst>
 </file>
 
@@ -811,7 +869,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,6 +933,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1043,7 +1108,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1212,7 +1277,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,6 +1486,24 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="index"/>
+      <sheetName val="correlation_colors"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1746,14 +1841,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D18" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{89256DDE-9554-499E-A7D9-CD9CC41B184F}">
-    <text>Should I winsorize it?</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0015E950-0C00-44DF-A022-5067B9A7E9E0}">
   <sheetPr>
@@ -1762,7 +1849,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1821,7 +1908,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2026,14 +2113,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C324394-3725-49AA-88D9-CE062D28E523}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C324394-3725-49AA-88D9-CE062D28E523}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2053,7 +2140,6 @@
       <c r="B1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="80"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -2063,7 +2149,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>22</v>
@@ -2250,6 +2336,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -2258,6 +2346,18 @@
       <c r="C20" s="10" t="s">
         <v>63</v>
       </c>
+      <c r="E20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="47">
+        <v>93</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="5">
+        <v>80</v>
+      </c>
       <c r="L20" s="35"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -2265,7 +2365,19 @@
         <v>0.01</v>
       </c>
       <c r="C21" s="9">
-        <v>-80.663570000000007</v>
+        <v>-166.69640000000001</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="48">
+        <v>93</v>
+      </c>
+      <c r="H21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
@@ -2273,16 +2385,29 @@
         <v>0.05</v>
       </c>
       <c r="C22" s="9">
-        <v>-4.4692429999999996</v>
-      </c>
+        <v>-14.417479999999999</v>
+      </c>
+      <c r="F22" s="28"/>
       <c r="L22" s="35"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="35">
         <v>0.1</v>
       </c>
       <c r="C23" s="9">
-        <v>-0.73104380000000002</v>
+        <v>-4.6349489999999998</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="28">
+        <v>1.2513000000000001</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="19">
+        <v>93</v>
       </c>
       <c r="L23" s="35"/>
     </row>
@@ -2291,12 +2416,19 @@
         <v>0.25</v>
       </c>
       <c r="C24" s="9">
-        <v>-0.25560250000000001</v>
+        <v>-1.3360289999999999</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="28">
+        <v>23.260300000000001</v>
       </c>
       <c r="L24" s="35"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C25" s="9"/>
+      <c r="F25" s="28"/>
       <c r="L25" s="35"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -2304,18 +2436,36 @@
         <v>0.5</v>
       </c>
       <c r="C26" s="9">
-        <v>9.4639000000000008E-3</v>
+        <v>0.63808260000000006</v>
+      </c>
+      <c r="E26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="28">
+        <v>541.04150000000004</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="28">
+        <v>-3.6497830000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="35">
         <v>0.75</v>
       </c>
       <c r="C28" s="9">
-        <v>0.48917830000000001</v>
+        <v>4.7886990000000003</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="49">
+        <v>33.000590000000003</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">
@@ -2323,7 +2473,7 @@
         <v>0.9</v>
       </c>
       <c r="C29" s="9">
-        <v>0.91621580000000002</v>
+        <v>15.169890000000001</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.35">
@@ -2331,7 +2481,7 @@
         <v>0.95</v>
       </c>
       <c r="C30" s="9">
-        <v>1.69503</v>
+        <v>31.69042</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2339,13 +2489,15 @@
         <v>0.99</v>
       </c>
       <c r="C31" s="46">
-        <v>789.47889999999995</v>
+        <v>87.77825</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H18:I18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2583,12 +2735,325 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="47.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="80" t="s">
+        <v>221</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="84"/>
+      <c r="C3" s="84"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="81" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="82" t="str">
+        <f>+VLOOKUP(B4,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: skill or accuracy in using hands/fingers</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C5" s="82" t="str">
+        <f>+VLOOKUP(B5,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: physical strength</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="82" t="str">
+        <f>+VLOOKUP(B6,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: physical stamina</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="82" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" s="82" t="str">
+        <f>+VLOOKUP(B8,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: dealing with people</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="82" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="82" t="str">
+        <f>+VLOOKUP(B9,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: working with a team</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="82" t="str">
+        <f>+VLOOKUP(B10,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: listening carefully to colleagues</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="82" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" s="82" t="str">
+        <f>+VLOOKUP(B11,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: making speeches/ presentations</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="82" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" s="82" t="str">
+        <f>+VLOOKUP(B12,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: persuading or influencing others</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="82" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="82" t="str">
+        <f>+VLOOKUP(B13,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: teaching people (individuals or groups)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="82" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="82" t="str">
+        <f>+VLOOKUP(B15,[1]!Table1[#Data],2,FALSE)</f>
+        <v>how often work involves short repetitive tasks</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="82" t="str">
+        <f>+VLOOKUP(B16,[1]!Table1[#Data],2,FALSE)</f>
+        <v>influence personally have on: quality standards work to</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="82" t="str">
+        <f>+VLOOKUP(B17,[1]!Table1[#Data],2,FALSE)</f>
+        <v>how much variety in job</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="82" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="82" t="str">
+        <f>+VLOOKUP(B18,[1]!Table1[#Data],2,FALSE)</f>
+        <v>Importance of planning own act, bigger=less routine</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="82"/>
+      <c r="C19" s="82"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="81" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="82" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="82" t="str">
+        <f>+VLOOKUP(B20,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: writing long documents</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="82" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="82" t="str">
+        <f>+VLOOKUP(B21,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: reading long documents</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="82" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="82" t="str">
+        <f>+VLOOKUP(B22,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: arithmetic (adding, subtracting, multiplying, divid</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="82" t="str">
+        <f>+VLOOKUP(B23,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: arithmetic involving fractions (decimals, percentag</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="82" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="82" t="str">
+        <f>+VLOOKUP(B24,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: advanced mathematics/ statistics (using calculator/</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="81" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="82" t="s">
+        <v>244</v>
+      </c>
+      <c r="C25" s="82" t="str">
+        <f>+VLOOKUP(B25,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: planning the activities of others</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="81" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="82" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" s="82" t="str">
+        <f>+VLOOKUP(B26,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: thinking of solutions to problems</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="C27" s="41" t="str">
+        <f>+VLOOKUP(B27,[1]!Table1[#Data],2,FALSE)</f>
+        <v>importance of: analysing complex problems in depth</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57CAF832-E4CD-4D78-919A-B2CAC1381075}">
   <dimension ref="B1:U15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G13" sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3196,8 +3661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DD79C6-8E03-4472-BA01-B1AB9175E2E7}">
   <dimension ref="B2:C65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3734,8 +4199,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D6"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4489,7 +4954,7 @@
   </sheetPr>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A21" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -5084,7 +5549,7 @@
   <dimension ref="B2:F32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5398,8 +5863,8 @@
   </sheetPr>
   <dimension ref="A1:AC15"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5911,8 +6376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F3C55B-20D0-4D01-AB90-788A157F68F3}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7073,8 +7538,8 @@
   </sheetPr>
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7245,7 +7710,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" s="79" t="s">
         <v>26</v>
       </c>
@@ -7254,14 +7719,14 @@
       <c r="D12" s="79"/>
       <c r="E12" s="79"/>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G13" s="78" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="78"/>
       <c r="I13" s="78"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
@@ -7287,7 +7752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -7316,7 +7781,7 @@
         <v>8.0096069126124061E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -7345,7 +7810,7 @@
         <v>8.2404717945099751E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="19" t="s">
         <v>10</v>
       </c>
@@ -7374,7 +7839,8 @@
         <v>8.992433008205325E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>140</v>
       </c>
@@ -7382,7 +7848,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -7399,7 +7865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>118</v>
       </c>
@@ -7410,7 +7876,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="23" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A23" s="79" t="s">
         <v>26</v>
       </c>
@@ -7419,14 +7886,14 @@
       <c r="D23" s="79"/>
       <c r="E23" s="79"/>
     </row>
-    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G24" s="78" t="s">
         <v>24</v>
       </c>
       <c r="H24" s="78"/>
       <c r="I24" s="78"/>
     </row>
-    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>8</v>
       </c>
@@ -7464,7 +7931,7 @@
         <v>0.24817665064047001</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -7505,7 +7972,7 @@
         <v>3.5119315719301103E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -7546,7 +8013,7 @@
         <v>9.3186362566577502E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="19" t="s">
         <v>10</v>
       </c>
@@ -7575,7 +8042,8 @@
         <v>0.38561453292854309</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>140</v>
       </c>
@@ -7583,7 +8051,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>19</v>
       </c>
@@ -7600,7 +8068,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
Got 2 eq solution sstandard errors
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8095FAF-6F48-4F3E-9275-C612C7BDD14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E923F7-8DAB-4DDD-9FC8-CF80CA41E2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="5" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -87,7 +87,7 @@
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
-    <comment ref="D42" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D45" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -895,10 +895,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
+    <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1139,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,6 +1278,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,7 +1324,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,7 +1879,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D42" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+  <threadedComment ref="D45" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
 </ThreadedComments>
@@ -1878,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7471085D-BC16-46A9-AF3A-D1F9FAE30012}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1971,19 +1982,19 @@
       <c r="A8" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="73">
         <v>-0.62474819000000004</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="73">
         <v>-0.72046911000000002</v>
       </c>
-      <c r="D8" s="88">
+      <c r="D8" s="73">
         <v>-0.84169570999999999</v>
       </c>
-      <c r="E8" s="88">
+      <c r="E8" s="73">
         <v>-0.57978885999999996</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="73">
         <v>0.99999998999999995</v>
       </c>
     </row>
@@ -1999,10 +2010,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2012,20 +2023,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2174,20 +2185,20 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
     </row>
     <row r="13" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G13" s="86" t="s">
+      <c r="G13" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
     </row>
     <row r="14" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
@@ -2341,20 +2352,20 @@
     </row>
     <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
     </row>
     <row r="24" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G24" s="86" t="s">
+      <c r="G24" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
@@ -2542,30 +2553,30 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="87" t="s">
+    <row r="34" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="87"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G35" s="86" t="s">
+      <c r="B34" s="88"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G35" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="87"/>
+      <c r="I35" s="87"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -2591,296 +2602,392 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="90">
         <v>0.38983157888076198</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="90">
         <v>0.77387006959986604</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="90">
         <v>0.132595645940602</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" ref="G37:G39" si="4">+C37/$B37</f>
+        <f t="shared" ref="G37" si="4">+C37/$B37</f>
         <v>1.2993343015929173</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" ref="H37:H39" si="5">+D37/$B37</f>
+        <f t="shared" ref="H37" si="5">+D37/$B37</f>
         <v>2.579359859183604</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" ref="I37:I39" si="6">+E37/$B37</f>
+        <f t="shared" ref="I37:I41" si="6">+E37/$B37</f>
         <v>0.44195001212354601</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B38" s="91">
+        <f>-G42</f>
+        <v>-3.27791808747964E-2</v>
+      </c>
+      <c r="C38" s="91">
+        <f t="shared" ref="C38:E38" si="7">-H42</f>
+        <v>-7.5396741976460305E-2</v>
+      </c>
+      <c r="D38" s="91">
+        <f t="shared" si="7"/>
+        <v>-0.115293505002319</v>
+      </c>
+      <c r="E38" s="91">
+        <f t="shared" si="7"/>
+        <v>-0.14196233908585501</v>
+      </c>
+      <c r="G38" s="18">
+        <f>+C39/$B39</f>
+        <v>1.7865633911582248</v>
+      </c>
+      <c r="H38" s="18">
+        <f>+D39/$B39</f>
+        <v>2.1717626166299819</v>
+      </c>
+      <c r="I38" s="18">
+        <f>+E39/$B39</f>
+        <v>0.23294604046745127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B39" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="90">
         <v>0.536012038389163</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D39" s="90">
         <v>0.65158108175637797</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="90">
         <v>6.9889421558501405E-2</v>
       </c>
-      <c r="G38" s="18">
-        <f t="shared" si="4"/>
-        <v>1.7865633911582248</v>
-      </c>
-      <c r="H38" s="18">
-        <f t="shared" si="5"/>
-        <v>2.1717626166299819</v>
-      </c>
-      <c r="I38" s="18">
-        <f t="shared" si="6"/>
-        <v>0.23294604046745127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="19" t="s">
+      <c r="G39" s="18">
+        <f>+C41/$B41</f>
+        <v>2.0941196035909679</v>
+      </c>
+      <c r="H39" s="18">
+        <f>+D41/$B41</f>
+        <v>1.8396516475591123</v>
+      </c>
+      <c r="I39" s="18">
+        <f>+E41/$B41</f>
+        <v>0.15281934113026216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B40" s="91">
+        <f>-G43</f>
+        <v>-3.5902339137002803E-2</v>
+      </c>
+      <c r="C40" s="91">
+        <f t="shared" ref="C40:E40" si="8">-H43</f>
+        <v>-8.7285450730600303E-2</v>
+      </c>
+      <c r="D40" s="91">
+        <f t="shared" si="8"/>
+        <v>-8.3582228841739506E-2</v>
+      </c>
+      <c r="E40" s="91">
+        <f t="shared" si="8"/>
+        <v>-9.8175524348070906E-2</v>
+      </c>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B41" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C41" s="90">
         <v>0.62828630817505104</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D41" s="90">
         <v>0.55193979369233104</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E41" s="90">
         <v>4.5849482279728501E-2</v>
       </c>
-      <c r="G39" s="18">
-        <f t="shared" si="4"/>
-        <v>2.0941196035909679</v>
-      </c>
-      <c r="H39" s="18">
-        <f t="shared" si="5"/>
-        <v>1.8396516475591123</v>
-      </c>
-      <c r="I39" s="18">
-        <f t="shared" si="6"/>
-        <v>0.15281934113026216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+    </row>
+    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="19"/>
+      <c r="B42" s="92">
+        <f>-G44</f>
+        <v>-3.5398027084865398E-2</v>
+      </c>
+      <c r="C42" s="92">
+        <f t="shared" ref="C42:E42" si="9">-H44</f>
+        <v>-8.8625088080741696E-2</v>
+      </c>
+      <c r="D42" s="92">
+        <f t="shared" si="9"/>
+        <v>-8.7677991056143698E-2</v>
+      </c>
+      <c r="E42" s="92">
+        <f t="shared" si="9"/>
+        <v>-7.5233432632621805E-2</v>
+      </c>
+      <c r="G42" s="18">
+        <v>3.27791808747964E-2</v>
+      </c>
+      <c r="H42" s="18">
+        <v>7.5396741976460305E-2</v>
+      </c>
+      <c r="I42" s="18">
+        <v>0.115293505002319</v>
+      </c>
+      <c r="J42">
+        <v>0.14196233908585501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>3.5902339137002803E-2</v>
+      </c>
+      <c r="H43">
+        <v>8.7285450730600303E-2</v>
+      </c>
+      <c r="I43">
+        <v>8.3582228841739506E-2</v>
+      </c>
+      <c r="J43">
+        <v>9.8175524348070906E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B44" s="54" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="G44">
+        <v>3.5398027084865398E-2</v>
+      </c>
+      <c r="H44">
+        <v>8.8625088080741696E-2</v>
+      </c>
+      <c r="I44">
+        <v>8.7677991056143698E-2</v>
+      </c>
+      <c r="J44">
+        <v>7.5233432632621805E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B45" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="55" t="s">
+      <c r="C45" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="55" t="s">
+      <c r="D45" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="55" t="s">
+      <c r="E45" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B46" s="1">
         <v>93</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="87" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="48" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="87"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G46" s="86" t="s">
+      <c r="B48" s="88"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G49" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="10" t="s">
+      <c r="H49" s="87"/>
+      <c r="I49" s="87"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G50" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H50" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I50" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B51" s="9">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C51" s="9">
         <v>0.376512905972681</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D51" s="9">
         <v>0.79002107522393805</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E51" s="9">
         <v>0.15027534446115601</v>
       </c>
-      <c r="G48" s="18">
-        <f t="shared" ref="G48:G50" si="7">+C48/$B48</f>
+      <c r="G51" s="18">
+        <f t="shared" ref="G51:G53" si="10">+C51/$B51</f>
         <v>1.373671978812486</v>
       </c>
-      <c r="H48" s="18">
-        <f t="shared" ref="H48:H50" si="8">+D48/$B48</f>
+      <c r="H51" s="18">
+        <f t="shared" ref="H51:H53" si="11">+D51/$B51</f>
         <v>2.882317701442024</v>
       </c>
-      <c r="I48" s="18">
-        <f t="shared" ref="I48:I50" si="9">+E48/$B48</f>
+      <c r="I51" s="18">
+        <f t="shared" ref="I51:I53" si="12">+E51/$B51</f>
         <v>0.54826548178845746</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B52" s="9">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C52" s="9">
         <v>0.581256120450657</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D52" s="9">
         <v>0.62356671376080797</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E52" s="9">
         <v>7.8971052048355805E-2</v>
       </c>
-      <c r="G49" s="18">
-        <f t="shared" si="7"/>
+      <c r="G52" s="18">
+        <f t="shared" si="10"/>
         <v>2.1206583692359722</v>
       </c>
-      <c r="H49" s="18">
-        <f t="shared" si="8"/>
+      <c r="H52" s="18">
+        <f t="shared" si="11"/>
         <v>2.2750245955063209</v>
       </c>
-      <c r="I49" s="18">
-        <f t="shared" si="9"/>
+      <c r="I52" s="18">
+        <f t="shared" si="12"/>
         <v>0.28811846716361922</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="19" t="s">
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B53" s="20">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C53" s="20">
         <v>0.51130203965422705</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D53" s="20">
         <v>0.61685941254475496</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E53" s="20">
         <v>0.13010063352593601</v>
       </c>
-      <c r="G50" s="18">
-        <f t="shared" si="7"/>
+      <c r="G53" s="18">
+        <f t="shared" si="10"/>
         <v>1.8654374748940057</v>
       </c>
-      <c r="H50" s="18">
-        <f t="shared" si="8"/>
+      <c r="H53" s="18">
+        <f t="shared" si="11"/>
         <v>2.2505536369075858</v>
       </c>
-      <c r="I50" s="18">
-        <f t="shared" si="9"/>
+      <c r="I53" s="18">
+        <f t="shared" si="12"/>
         <v>0.47465994356458474</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="64" t="s">
+      <c r="B55" s="64" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B56" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="55" t="s">
+      <c r="C56" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="55" t="s">
+      <c r="D56" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="55" t="s">
+      <c r="E56" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B57" s="4">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="G35:I35"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="G49:I49"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A12:E12"/>
@@ -2949,7 +3056,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37:G39">
+  <conditionalFormatting sqref="G37:G40 G42">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2959,7 +3066,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37:H39">
+  <conditionalFormatting sqref="H37:H40 H42">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2969,7 +3076,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:I39">
+  <conditionalFormatting sqref="I37:I40 I42">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2979,7 +3086,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48:G50">
+  <conditionalFormatting sqref="G51:G53">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2989,7 +3096,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48:H50">
+  <conditionalFormatting sqref="H51:H53">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2999,7 +3106,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:I50">
+  <conditionalFormatting sqref="I51:I53">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3071,20 +3178,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3481,8 +3588,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3680,12 +3787,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4270,66 +4377,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="N1" s="73" t="s">
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="N1" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="T1" s="73" t="s">
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="T1" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="N2" s="74" t="s">
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="N2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="T2" s="74" t="s">
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="T2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5361,10 +5468,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -5899,13 +6006,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6019,12 +6126,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6323,12 +6430,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -6662,13 +6769,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -6906,13 +7013,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -6940,13 +7047,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7208,13 +7315,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="80" t="s">
+      <c r="A43" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -7582,36 +7689,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="81"/>
-      <c r="V3" s="81"/>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="81"/>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
-      <c r="AB3" s="81"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8095,35 +8202,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="82" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="83" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Finished 2-equation standard errors
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E923F7-8DAB-4DDD-9FC8-CF80CA41E2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF4813-25DE-4B9F-A044-2E75399FBAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="5" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -2013,7 +2013,7 @@
   <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2677,6 +2677,7 @@
       <c r="E39" s="90">
         <v>6.9889421558501405E-2</v>
       </c>
+      <c r="F39" s="18"/>
       <c r="G39" s="18">
         <f>+C41/$B41</f>
         <v>2.0941196035909679</v>
@@ -2727,6 +2728,7 @@
       <c r="E41" s="90">
         <v>4.5849482279728501E-2</v>
       </c>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="19"/>

</xml_diff>

<commit_message>
Wrote standard errors for 3 equation solution
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8095FAF-6F48-4F3E-9275-C612C7BDD14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF4813-25DE-4B9F-A044-2E75399FBAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="5" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -87,7 +87,7 @@
     <author>tc={134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}</author>
   </authors>
   <commentList>
-    <comment ref="D42" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+    <comment ref="D45" authorId="0" shapeId="0" xr:uid="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -895,10 +895,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000_);\(0.0000\)"/>
+    <numFmt numFmtId="167" formatCode="0.000_);\(0.000\)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1139,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1277,6 +1278,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,7 +1324,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1868,7 +1879,7 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D42" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
+  <threadedComment ref="D45" dT="2023-05-04T15:19:28.63" personId="{F8FA700A-AE49-4429-93AD-D984B9D4E946}" id="{134ADD85-417C-4FE4-8D98-C9A6AB9E32ED}">
     <text>Should I winsorize it?</text>
   </threadedComment>
 </ThreadedComments>
@@ -1878,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7471085D-BC16-46A9-AF3A-D1F9FAE30012}">
   <dimension ref="A2:F9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1971,19 +1982,19 @@
       <c r="A8" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="73">
         <v>-0.62474819000000004</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="73">
         <v>-0.72046911000000002</v>
       </c>
-      <c r="D8" s="88">
+      <c r="D8" s="73">
         <v>-0.84169570999999999</v>
       </c>
-      <c r="E8" s="88">
+      <c r="E8" s="73">
         <v>-0.57978885999999996</v>
       </c>
-      <c r="F8" s="88">
+      <c r="F8" s="73">
         <v>0.99999998999999995</v>
       </c>
     </row>
@@ -1999,10 +2010,10 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2012,20 +2023,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2174,20 +2185,20 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="87" t="s">
+      <c r="A12" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
     </row>
     <row r="13" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G13" s="86" t="s">
+      <c r="G13" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
     </row>
     <row r="14" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
@@ -2341,20 +2352,20 @@
     </row>
     <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="87" t="s">
+      <c r="A23" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
     </row>
     <row r="24" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G24" s="86" t="s">
+      <c r="G24" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="86"/>
-      <c r="I24" s="86"/>
+      <c r="H24" s="87"/>
+      <c r="I24" s="87"/>
     </row>
     <row r="25" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
@@ -2542,30 +2553,30 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="87" t="s">
+    <row r="34" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="87"/>
-      <c r="C34" s="87"/>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G35" s="86" t="s">
+      <c r="B34" s="88"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="88"/>
+    </row>
+    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G35" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H35" s="87"/>
+      <c r="I35" s="87"/>
+    </row>
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
         <v>8</v>
       </c>
@@ -2591,296 +2602,394 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="90">
         <v>0.38983157888076198</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="90">
         <v>0.77387006959986604</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="90">
         <v>0.132595645940602</v>
       </c>
       <c r="G37" s="18">
-        <f t="shared" ref="G37:G39" si="4">+C37/$B37</f>
+        <f t="shared" ref="G37" si="4">+C37/$B37</f>
         <v>1.2993343015929173</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" ref="H37:H39" si="5">+D37/$B37</f>
+        <f t="shared" ref="H37" si="5">+D37/$B37</f>
         <v>2.579359859183604</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" ref="I37:I39" si="6">+E37/$B37</f>
+        <f t="shared" ref="I37:I41" si="6">+E37/$B37</f>
         <v>0.44195001212354601</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B38" s="91">
+        <f>-G42</f>
+        <v>-3.27791808747964E-2</v>
+      </c>
+      <c r="C38" s="91">
+        <f t="shared" ref="C38:E38" si="7">-H42</f>
+        <v>-7.5396741976460305E-2</v>
+      </c>
+      <c r="D38" s="91">
+        <f t="shared" si="7"/>
+        <v>-0.115293505002319</v>
+      </c>
+      <c r="E38" s="91">
+        <f t="shared" si="7"/>
+        <v>-0.14196233908585501</v>
+      </c>
+      <c r="G38" s="18">
+        <f>+C39/$B39</f>
+        <v>1.7865633911582248</v>
+      </c>
+      <c r="H38" s="18">
+        <f>+D39/$B39</f>
+        <v>2.1717626166299819</v>
+      </c>
+      <c r="I38" s="18">
+        <f>+E39/$B39</f>
+        <v>0.23294604046745127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B39" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C39" s="90">
         <v>0.536012038389163</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D39" s="90">
         <v>0.65158108175637797</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E39" s="90">
         <v>6.9889421558501405E-2</v>
       </c>
-      <c r="G38" s="18">
-        <f t="shared" si="4"/>
-        <v>1.7865633911582248</v>
-      </c>
-      <c r="H38" s="18">
-        <f t="shared" si="5"/>
-        <v>2.1717626166299819</v>
-      </c>
-      <c r="I38" s="18">
-        <f t="shared" si="6"/>
-        <v>0.23294604046745127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="19" t="s">
+      <c r="F39" s="18"/>
+      <c r="G39" s="18">
+        <f>+C41/$B41</f>
+        <v>2.0941196035909679</v>
+      </c>
+      <c r="H39" s="18">
+        <f>+D41/$B41</f>
+        <v>1.8396516475591123</v>
+      </c>
+      <c r="I39" s="18">
+        <f>+E41/$B41</f>
+        <v>0.15281934113026216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B40" s="91">
+        <f>-G43</f>
+        <v>-3.5902339137002803E-2</v>
+      </c>
+      <c r="C40" s="91">
+        <f t="shared" ref="C40:E40" si="8">-H43</f>
+        <v>-8.7285450730600303E-2</v>
+      </c>
+      <c r="D40" s="91">
+        <f t="shared" si="8"/>
+        <v>-8.3582228841739506E-2</v>
+      </c>
+      <c r="E40" s="91">
+        <f t="shared" si="8"/>
+        <v>-9.8175524348070906E-2</v>
+      </c>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B41" s="90">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C41" s="90">
         <v>0.62828630817505104</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D41" s="90">
         <v>0.55193979369233104</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E41" s="90">
         <v>4.5849482279728501E-2</v>
       </c>
-      <c r="G39" s="18">
-        <f t="shared" si="4"/>
-        <v>2.0941196035909679</v>
-      </c>
-      <c r="H39" s="18">
-        <f t="shared" si="5"/>
-        <v>1.8396516475591123</v>
-      </c>
-      <c r="I39" s="18">
-        <f t="shared" si="6"/>
-        <v>0.15281934113026216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="19"/>
+      <c r="B42" s="92">
+        <f>-G44</f>
+        <v>-3.5398027084865398E-2</v>
+      </c>
+      <c r="C42" s="92">
+        <f t="shared" ref="C42:E42" si="9">-H44</f>
+        <v>-8.8625088080741696E-2</v>
+      </c>
+      <c r="D42" s="92">
+        <f t="shared" si="9"/>
+        <v>-8.7677991056143698E-2</v>
+      </c>
+      <c r="E42" s="92">
+        <f t="shared" si="9"/>
+        <v>-7.5233432632621805E-2</v>
+      </c>
+      <c r="G42" s="18">
+        <v>3.27791808747964E-2</v>
+      </c>
+      <c r="H42" s="18">
+        <v>7.5396741976460305E-2</v>
+      </c>
+      <c r="I42" s="18">
+        <v>0.115293505002319</v>
+      </c>
+      <c r="J42">
+        <v>0.14196233908585501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>3.5902339137002803E-2</v>
+      </c>
+      <c r="H43">
+        <v>8.7285450730600303E-2</v>
+      </c>
+      <c r="I43">
+        <v>8.3582228841739506E-2</v>
+      </c>
+      <c r="J43">
+        <v>9.8175524348070906E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B44" s="54" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
+      <c r="G44">
+        <v>3.5398027084865398E-2</v>
+      </c>
+      <c r="H44">
+        <v>8.8625088080741696E-2</v>
+      </c>
+      <c r="I44">
+        <v>8.7677991056143698E-2</v>
+      </c>
+      <c r="J44">
+        <v>7.5233432632621805E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B45" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="55" t="s">
+      <c r="C45" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="55" t="s">
+      <c r="D45" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="55" t="s">
+      <c r="E45" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B46" s="1">
         <v>93</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="45" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="87" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="48" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B45" s="87"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G46" s="86" t="s">
+      <c r="B48" s="88"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="G49" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="10" t="s">
+      <c r="H49" s="87"/>
+      <c r="I49" s="87"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G50" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H47" s="8" t="s">
+      <c r="H50" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I47" s="8" t="s">
+      <c r="I50" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B51" s="9">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C51" s="9">
         <v>0.376512905972681</v>
       </c>
-      <c r="D48" s="9">
+      <c r="D51" s="9">
         <v>0.79002107522393805</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E51" s="9">
         <v>0.15027534446115601</v>
       </c>
-      <c r="G48" s="18">
-        <f t="shared" ref="G48:G50" si="7">+C48/$B48</f>
+      <c r="G51" s="18">
+        <f t="shared" ref="G51:G53" si="10">+C51/$B51</f>
         <v>1.373671978812486</v>
       </c>
-      <c r="H48" s="18">
-        <f t="shared" ref="H48:H50" si="8">+D48/$B48</f>
+      <c r="H51" s="18">
+        <f t="shared" ref="H51:H53" si="11">+D51/$B51</f>
         <v>2.882317701442024</v>
       </c>
-      <c r="I48" s="18">
-        <f t="shared" ref="I48:I50" si="9">+E48/$B48</f>
+      <c r="I51" s="18">
+        <f t="shared" ref="I51:I53" si="12">+E51/$B51</f>
         <v>0.54826548178845746</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>9</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B52" s="9">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C52" s="9">
         <v>0.581256120450657</v>
       </c>
-      <c r="D49" s="9">
+      <c r="D52" s="9">
         <v>0.62356671376080797</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E52" s="9">
         <v>7.8971052048355805E-2</v>
       </c>
-      <c r="G49" s="18">
-        <f t="shared" si="7"/>
+      <c r="G52" s="18">
+        <f t="shared" si="10"/>
         <v>2.1206583692359722</v>
       </c>
-      <c r="H49" s="18">
-        <f t="shared" si="8"/>
+      <c r="H52" s="18">
+        <f t="shared" si="11"/>
         <v>2.2750245955063209</v>
       </c>
-      <c r="I49" s="18">
-        <f t="shared" si="9"/>
+      <c r="I52" s="18">
+        <f t="shared" si="12"/>
         <v>0.28811846716361922</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="19" t="s">
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B53" s="20">
         <v>0.27409229552616299</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C53" s="20">
         <v>0.51130203965422705</v>
       </c>
-      <c r="D50" s="20">
+      <c r="D53" s="20">
         <v>0.61685941254475496</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E53" s="20">
         <v>0.13010063352593601</v>
       </c>
-      <c r="G50" s="18">
-        <f t="shared" si="7"/>
+      <c r="G53" s="18">
+        <f t="shared" si="10"/>
         <v>1.8654374748940057</v>
       </c>
-      <c r="H50" s="18">
-        <f t="shared" si="8"/>
+      <c r="H53" s="18">
+        <f t="shared" si="11"/>
         <v>2.2505536369075858</v>
       </c>
-      <c r="I50" s="18">
-        <f t="shared" si="9"/>
+      <c r="I53" s="18">
+        <f t="shared" si="12"/>
         <v>0.47465994356458474</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="64" t="s">
+      <c r="B55" s="64" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="4" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="55" t="s">
+      <c r="B56" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="55" t="s">
+      <c r="C56" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="55" t="s">
+      <c r="D56" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="55" t="s">
+      <c r="E56" s="55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="4" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B57" s="4">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="G35:I35"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="G49:I49"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A12:E12"/>
@@ -2949,7 +3058,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G37:G39">
+  <conditionalFormatting sqref="G37:G40 G42">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2959,7 +3068,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37:H39">
+  <conditionalFormatting sqref="H37:H40 H42">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2969,7 +3078,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:I39">
+  <conditionalFormatting sqref="I37:I40 I42">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2979,7 +3088,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48:G50">
+  <conditionalFormatting sqref="G51:G53">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2989,7 +3098,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48:H50">
+  <conditionalFormatting sqref="H51:H53">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2999,7 +3108,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I48:I50">
+  <conditionalFormatting sqref="I51:I53">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3071,20 +3180,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3481,8 +3590,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3680,12 +3789,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4270,66 +4379,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="N1" s="73" t="s">
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="N1" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="73"/>
-      <c r="P1" s="73"/>
-      <c r="Q1" s="73"/>
-      <c r="R1" s="73"/>
-      <c r="T1" s="73" t="s">
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="T1" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="73"/>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="N2" s="74" t="s">
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="N2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="T2" s="74" t="s">
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
+      <c r="R2" s="75"/>
+      <c r="T2" s="75" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5361,10 +5470,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="77" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -5899,13 +6008,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6019,12 +6128,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6323,12 +6432,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
+      <c r="B37" s="79"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -6662,13 +6771,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -6906,13 +7015,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="80" t="s">
+      <c r="A21" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -6940,13 +7049,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
+      <c r="B25" s="80"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7208,13 +7317,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="80" t="s">
+      <c r="A43" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="80"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="81"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="81"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -7582,36 +7691,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="81" t="s">
+      <c r="A3" s="82" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
-      <c r="T3" s="81"/>
-      <c r="U3" s="81"/>
-      <c r="V3" s="81"/>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="81"/>
-      <c r="Z3" s="81"/>
-      <c r="AA3" s="81"/>
-      <c r="AB3" s="81"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8095,35 +8204,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="85" t="s">
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="82" t="s">
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="83" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="83"/>
-      <c r="S4" s="83"/>
-      <c r="T4" s="83"/>
-      <c r="U4" s="83"/>
-      <c r="V4" s="83"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="84"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="84"/>
+      <c r="U4" s="84"/>
+      <c r="V4" s="84"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Commented code two equation version
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_6_22.xlsx
+++ b/results/tables/final_tables_6_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADF4813-25DE-4B9F-A044-2E75399FBAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C7A3E5-6360-4DDA-8838-00B72988985B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="5" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -1140,7 +1140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1279,6 +1279,15 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,16 +1331,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2012,7 +2011,7 @@
   </sheetPr>
   <dimension ref="A1:O57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -2023,20 +2022,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="87" t="s">
+      <c r="G2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2185,20 +2184,20 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="91"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="91"/>
     </row>
     <row r="13" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G13" s="87" t="s">
+      <c r="G13" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
     </row>
     <row r="14" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
@@ -2352,20 +2351,20 @@
     </row>
     <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="88" t="s">
+      <c r="A23" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="88"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
     </row>
     <row r="24" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G24" s="87" t="s">
+      <c r="G24" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
     </row>
     <row r="25" spans="1:15" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
@@ -2561,20 +2560,20 @@
       <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="88" t="s">
+      <c r="A34" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="88"/>
-      <c r="C34" s="88"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="91"/>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G35" s="87" t="s">
+      <c r="G35" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
@@ -2606,16 +2605,16 @@
       <c r="A37" t="s">
         <v>93</v>
       </c>
-      <c r="B37" s="90">
+      <c r="B37" s="74">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C37" s="90">
+      <c r="C37" s="74">
         <v>0.38983157888076198</v>
       </c>
-      <c r="D37" s="90">
+      <c r="D37" s="74">
         <v>0.77387006959986604</v>
       </c>
-      <c r="E37" s="90">
+      <c r="E37" s="74">
         <v>0.132595645940602</v>
       </c>
       <c r="G37" s="18">
@@ -2627,24 +2626,24 @@
         <v>2.579359859183604</v>
       </c>
       <c r="I37" s="18">
-        <f t="shared" ref="I37:I41" si="6">+E37/$B37</f>
+        <f t="shared" ref="I37" si="6">+E37/$B37</f>
         <v>0.44195001212354601</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B38" s="91">
+      <c r="B38" s="75">
         <f>-G42</f>
         <v>-3.27791808747964E-2</v>
       </c>
-      <c r="C38" s="91">
+      <c r="C38" s="75">
         <f t="shared" ref="C38:E38" si="7">-H42</f>
         <v>-7.5396741976460305E-2</v>
       </c>
-      <c r="D38" s="91">
+      <c r="D38" s="75">
         <f t="shared" si="7"/>
         <v>-0.115293505002319</v>
       </c>
-      <c r="E38" s="91">
+      <c r="E38" s="75">
         <f t="shared" si="7"/>
         <v>-0.14196233908585501</v>
       </c>
@@ -2665,16 +2664,16 @@
       <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="90">
+      <c r="B39" s="74">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C39" s="90">
+      <c r="C39" s="74">
         <v>0.536012038389163</v>
       </c>
-      <c r="D39" s="90">
+      <c r="D39" s="74">
         <v>0.65158108175637797</v>
       </c>
-      <c r="E39" s="90">
+      <c r="E39" s="74">
         <v>6.9889421558501405E-2</v>
       </c>
       <c r="F39" s="18"/>
@@ -2692,19 +2691,19 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B40" s="91">
+      <c r="B40" s="75">
         <f>-G43</f>
         <v>-3.5902339137002803E-2</v>
       </c>
-      <c r="C40" s="91">
+      <c r="C40" s="75">
         <f t="shared" ref="C40:E40" si="8">-H43</f>
         <v>-8.7285450730600303E-2</v>
       </c>
-      <c r="D40" s="91">
+      <c r="D40" s="75">
         <f t="shared" si="8"/>
         <v>-8.3582228841739506E-2</v>
       </c>
-      <c r="E40" s="91">
+      <c r="E40" s="75">
         <f t="shared" si="8"/>
         <v>-9.8175524348070906E-2</v>
       </c>
@@ -2713,38 +2712,38 @@
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="89" t="s">
+      <c r="A41" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="90">
+      <c r="B41" s="74">
         <v>0.30002408033317401</v>
       </c>
-      <c r="C41" s="90">
+      <c r="C41" s="74">
         <v>0.62828630817505104</v>
       </c>
-      <c r="D41" s="90">
+      <c r="D41" s="74">
         <v>0.55193979369233104</v>
       </c>
-      <c r="E41" s="90">
+      <c r="E41" s="74">
         <v>4.5849482279728501E-2</v>
       </c>
       <c r="F41" s="18"/>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="19"/>
-      <c r="B42" s="92">
+      <c r="B42" s="76">
         <f>-G44</f>
         <v>-3.5398027084865398E-2</v>
       </c>
-      <c r="C42" s="92">
+      <c r="C42" s="76">
         <f t="shared" ref="C42:E42" si="9">-H44</f>
         <v>-8.8625088080741696E-2</v>
       </c>
-      <c r="D42" s="92">
+      <c r="D42" s="76">
         <f t="shared" si="9"/>
         <v>-8.7677991056143698E-2</v>
       </c>
-      <c r="E42" s="92">
+      <c r="E42" s="76">
         <f t="shared" si="9"/>
         <v>-7.5233432632621805E-2</v>
       </c>
@@ -2824,20 +2823,20 @@
       <c r="E46" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="88" t="s">
+      <c r="A48" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="88"/>
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
+      <c r="B48" s="91"/>
+      <c r="C48" s="91"/>
+      <c r="D48" s="91"/>
+      <c r="E48" s="91"/>
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G49" s="87" t="s">
+      <c r="G49" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="87"/>
-      <c r="I49" s="87"/>
+      <c r="H49" s="90"/>
+      <c r="I49" s="90"/>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="10" t="s">
@@ -3180,20 +3179,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3590,8 +3589,8 @@
       <c r="E18" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="77"/>
-      <c r="I18" s="77"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
       <c r="L18" s="35"/>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -3789,12 +3788,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4379,66 +4378,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="77" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="N1" s="74" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="N1" s="77" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="T1" s="74" t="s">
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="T1" s="77" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="75" t="s">
+      <c r="H2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="N2" s="75" t="s">
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="N2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="T2" s="75" t="s">
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="T2" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79"/>
+      <c r="X2" s="79"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5470,10 +5469,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="80" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="77"/>
+      <c r="C2" s="80"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -6008,13 +6007,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6128,12 +6127,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="79"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -6432,12 +6431,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="79"/>
-      <c r="C37" s="79"/>
-      <c r="D37" s="79"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -6771,13 +6770,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="83" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -7015,13 +7014,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -7049,13 +7048,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="80" t="s">
+      <c r="A25" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -7317,13 +7316,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="81"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
+      <c r="B43" s="84"/>
+      <c r="C43" s="84"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -7691,36 +7690,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
-      <c r="P3" s="82"/>
-      <c r="Q3" s="82"/>
-      <c r="R3" s="82"/>
-      <c r="S3" s="82"/>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="82"/>
-      <c r="W3" s="82"/>
-      <c r="X3" s="82"/>
-      <c r="Y3" s="82"/>
-      <c r="Z3" s="82"/>
-      <c r="AA3" s="82"/>
-      <c r="AB3" s="82"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="85"/>
+      <c r="AB3" s="85"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -8204,35 +8203,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="83" t="s">
+      <c r="F4" s="89"/>
+      <c r="G4" s="89"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="89"/>
+      <c r="K4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84" t="s">
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="84"/>
-      <c r="U4" s="84"/>
-      <c r="V4" s="84"/>
+      <c r="P4" s="87"/>
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="87"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>